<commit_message>
Adding PRIMERAY KEYS to RATES Table + implementing POST request
</commit_message>
<xml_diff>
--- a/providers/app/flask-app/in/rates.xlsx
+++ b/providers/app/flask-app/in/rates.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t xml:space="preserve">Product</t>
   </si>
@@ -34,10 +34,10 @@
     <t xml:space="preserve">Navel</t>
   </si>
   <si>
+    <t xml:space="preserve">Blood</t>
+  </si>
+  <si>
     <t xml:space="preserve">All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blood</t>
   </si>
   <si>
     <t xml:space="preserve">Mandarin</t>
@@ -70,6 +70,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -140,12 +141,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -155,10 +156,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -182,21 +183,21 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>4</v>
+        <v>100</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>112</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -207,7 +208,7 @@
         <v>104</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -218,7 +219,7 @@
         <v>84</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -229,7 +230,7 @@
         <v>92</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -240,7 +241,7 @@
         <v>113</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -251,7 +252,7 @@
         <v>88</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -262,7 +263,7 @@
         <v>87</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -307,6 +308,17 @@
       </c>
       <c r="C13" s="0" t="n">
         <v>45</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implementing GET /rates. WORKING :)
</commit_message>
<xml_diff>
--- a/providers/app/flask-app/in/rates.xlsx
+++ b/providers/app/flask-app/in/rates.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
   <si>
     <t xml:space="preserve">Product</t>
   </si>
@@ -34,10 +34,10 @@
     <t xml:space="preserve">Navel</t>
   </si>
   <si>
+    <t xml:space="preserve">All</t>
+  </si>
+  <si>
     <t xml:space="preserve">Blood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All</t>
   </si>
   <si>
     <t xml:space="preserve">Mandarin</t>
@@ -70,7 +70,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -141,12 +140,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -156,10 +155,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -183,21 +182,21 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>3</v>
+        <v>93</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>112</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -208,7 +207,7 @@
         <v>104</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -219,7 +218,7 @@
         <v>84</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -230,7 +229,7 @@
         <v>92</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -241,7 +240,7 @@
         <v>113</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -252,7 +251,7 @@
         <v>88</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -263,7 +262,7 @@
         <v>87</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -308,17 +307,6 @@
       </c>
       <c r="C13" s="0" t="n">
         <v>45</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>114</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>